<commit_message>
Added Mime Types for Allure Attachements
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel Files/testGoogle.xlsx
+++ b/src/test/resources/Excel Files/testGoogle.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="testGoogle" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -33,41 +33,17 @@
     <t>Gladson</t>
   </si>
   <si>
-    <t>Antony</t>
-  </si>
-  <si>
     <t>TC_001</t>
   </si>
   <si>
-    <t>TC_002</t>
-  </si>
-  <si>
     <t>Gladson_Password</t>
-  </si>
-  <si>
-    <t>Antony_Password</t>
-  </si>
-  <si>
-    <t>TC_003</t>
-  </si>
-  <si>
-    <t>Glady</t>
-  </si>
-  <si>
-    <t>Glady_Password</t>
-  </si>
-  <si>
-    <t>TC_004</t>
-  </si>
-  <si>
-    <t>GladyBLAZE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,7 +165,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -224,7 +200,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -401,29 +377,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.25" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" hidden="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,50 +410,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
+    <row r="3" spans="1:3"/>
+    <row r="4" spans="1:3"/>
+    <row r="5" spans="1:3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Webelement Capture Method for Allure Report Attachment
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel Files/testGoogle.xlsx
+++ b/src/test/resources/Excel Files/testGoogle.xlsx
@@ -377,7 +377,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -388,7 +388,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD5"/>
+      <selection activeCell="A3" sqref="A3:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -421,9 +421,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3"/>
-    <row r="4" spans="1:3"/>
-    <row r="5" spans="1:3"/>
+    <row r="3" spans="1:3" hidden="1"/>
+    <row r="4" spans="1:3" hidden="1"/>
+    <row r="5" spans="1:3" hidden="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Chrome_Headless as a Browser Option. Updated Webdriver to 3.4.0. Updated WebDriverManger to 1.7.1
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel Files/testGoogle.xlsx
+++ b/src/test/resources/Excel Files/testGoogle.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="11760"/>
   </bookViews>
@@ -10,8 +10,8 @@
     <sheet name="testGoogle" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -42,8 +42,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,21 +377,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -399,7 +399,7 @@
     <col min="4" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,7 +410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -421,9 +421,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1"/>
-    <row r="4" spans="1:3" hidden="1"/>
-    <row r="5" spans="1:3" hidden="1"/>
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Support for XLS-TestNg DataProvider, Updated to Selenium 3.5.5, Added ExplicitWaiting Class
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel Files/testGoogle.xlsx
+++ b/src/test/resources/Excel Files/testGoogle.xlsx
@@ -2,14 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Java\Eclipse Workspace\WebAppllWDM\src\test\resources\Excel Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20700" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11865"/>
   </bookViews>
   <sheets>
-    <sheet name="testGoogle" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,10 +35,10 @@
     <t>Password</t>
   </si>
   <si>
+    <t>TC_001</t>
+  </si>
+  <si>
     <t>Gladson</t>
-  </si>
-  <si>
-    <t>TC_001</t>
   </si>
   <si>
     <t>Gladson_Password</t>
@@ -165,7 +170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -200,7 +205,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -385,18 +390,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" hidden="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -412,20 +416,16 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>